<commit_message>
Setores das empresas da B3
</commit_message>
<xml_diff>
--- a/Covenants/Setores das empresas B3.xlsx
+++ b/Covenants/Setores das empresas B3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\{estudos}\Python\Estudos-Python\Covenants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0032A41D-991A-4119-9E7F-D5B4D274E849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CBDF17-6C42-41BE-8466-CBA99366699A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D3E51146-1430-4549-80ED-4A3F606CC1EE}"/>
   </bookViews>
@@ -2705,9 +2705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AE7DB7-2DE2-480D-BB8F-D7FD3739125F}">
   <dimension ref="A1:C376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A359" workbookViewId="0">
-      <selection activeCell="E364" sqref="E364"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>